<commit_message>
Separate generic unix setup from docker/podman specific set up
</commit_message>
<xml_diff>
--- a/90_Misc/time_log.xlsx
+++ b/90_Misc/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/move_network/90_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC306E5-9404-FC4F-8849-8F5316ED117D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678B0705-C14C-8A48-8A6A-45F28262E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1340" windowWidth="21020" windowHeight="17460" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="4" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -144,7 +144,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -208,7 +243,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45774.431883680554" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45774.564440393522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Log"/>
   </cacheSource>
@@ -217,10 +252,10 @@
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-04-27T00:00:00" maxDate="2025-04-28T00:00:00"/>
     </cacheField>
     <cacheField name="Start" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T10:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T13:30:00"/>
     </cacheField>
     <cacheField name="End" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T14:00:00" maxDate="1899-12-30T14:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T11:45:00" maxDate="1899-12-30T15:00:00"/>
     </cacheField>
     <cacheField name="Project" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -232,7 +267,7 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.5" maxValue="1.7499999999999991"/>
     </cacheField>
     <cacheField name="Week" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="18" count="2">
@@ -250,16 +285,156 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
   <r>
     <d v="2025-04-27T00:00:00"/>
     <d v="1899-12-30T10:00:00"/>
-    <d v="1899-12-30T14:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
     <s v="move_network"/>
     <n v="12"/>
     <m/>
-    <n v="4"/>
+    <n v="1.7499999999999991"/>
     <x v="0"/>
+  </r>
+  <r>
+    <d v="2025-04-27T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <s v="move_network"/>
+    <n v="12"/>
+    <m/>
+    <n v="1.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
   </r>
   <r>
     <m/>
@@ -275,7 +450,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -311,16 +486,16 @@
     <dataField name="Sum of Time" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="6">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="9">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="1">
@@ -329,10 +504,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -679,7 +854,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +914,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C2" s="6">
-        <v>0.58333333333333337</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
@@ -749,7 +924,7 @@
       </c>
       <c r="G2" s="7">
         <f>(C2-B2)*24</f>
-        <v>4</v>
+        <v>1.7499999999999991</v>
       </c>
       <c r="H2" s="1">
         <f>WEEKNUM(A2)</f>
@@ -759,16 +934,40 @@
         <v>18</v>
       </c>
       <c r="K2" s="10">
-        <v>4</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <f>DATE(2025,4,27)</f>
+        <v>45774</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7">
+        <f>(C3-B3)*24</f>
+        <v>1.5</v>
+      </c>
+      <c r="H3" s="1">
+        <f>WEEKNUM(A3)</f>
+        <v>18</v>
+      </c>
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="10">
-        <v>4</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="L3" s="8"/>
     </row>

</xml_diff>

<commit_message>
Reconfigure 11 scripts to use Podman instead of Docker
</commit_message>
<xml_diff>
--- a/90_Misc/time_log.xlsx
+++ b/90_Misc/time_log.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/move_network/90_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678B0705-C14C-8A48-8A6A-45F28262E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD609019-87F7-204D-B143-BEFFE06262C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1340" windowWidth="21020" windowHeight="17460" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
+    <workbookView xWindow="-35840" yWindow="500" windowWidth="13080" windowHeight="17400" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -139,54 +139,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -450,7 +407,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -486,16 +443,16 @@
     <dataField name="Sum of Time" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="11">
+    <format dxfId="5">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="3">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="1">
@@ -504,10 +461,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -854,7 +811,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,7 +890,7 @@
       <c r="J2" s="9">
         <v>18</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="8">
         <v>3.2499999999999991</v>
       </c>
       <c r="L2" s="8"/>
@@ -966,7 +923,7 @@
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <v>3.2499999999999991</v>
       </c>
       <c r="L3" s="8"/>

</xml_diff>

<commit_message>
Build pypi server container
</commit_message>
<xml_diff>
--- a/90_Misc/time_log.xlsx
+++ b/90_Misc/time_log.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/move_network/90_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD609019-87F7-204D-B143-BEFFE06262C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653C9842-33EC-5E47-AA99-DB388801F111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="500" windowWidth="13080" windowHeight="17400" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
+    <workbookView xWindow="-30000" yWindow="1760" windowWidth="20000" windowHeight="18760" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="4" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -139,11 +139,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -200,7 +243,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45774.564440393522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45787.496661111109" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Log"/>
   </cacheSource>
@@ -212,7 +255,7 @@
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T13:30:00"/>
     </cacheField>
     <cacheField name="End" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T11:45:00" maxDate="1899-12-30T15:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T11:45:00" maxDate="1899-12-30T16:00:00"/>
     </cacheField>
     <cacheField name="Project" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -224,7 +267,7 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.5" maxValue="1.7499999999999991"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.7499999999999991" maxValue="3.9999999999999991"/>
     </cacheField>
     <cacheField name="Week" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="18" count="2">
@@ -256,22 +299,22 @@
   <r>
     <d v="2025-04-27T00:00:00"/>
     <d v="1899-12-30T13:30:00"/>
-    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T15:15:00"/>
     <s v="move_network"/>
     <n v="12"/>
     <m/>
-    <n v="1.5"/>
+    <n v="1.7499999999999991"/>
     <x v="0"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <d v="2025-04-27T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <s v="move_network"/>
+    <n v="12"/>
+    <m/>
+    <n v="3.9999999999999991"/>
+    <x v="0"/>
   </r>
   <r>
     <m/>
@@ -407,7 +450,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -443,16 +486,16 @@
     <dataField name="Sum of Time" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="5">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="9">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="1">
@@ -461,10 +504,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -811,7 +854,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,8 +933,8 @@
       <c r="J2" s="9">
         <v>18</v>
       </c>
-      <c r="K2" s="8">
-        <v>3.2499999999999991</v>
+      <c r="K2" s="10">
+        <v>7.4999999999999973</v>
       </c>
       <c r="L2" s="8"/>
     </row>
@@ -904,7 +947,7 @@
         <v>0.5625</v>
       </c>
       <c r="C3" s="6">
-        <v>0.625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -914,7 +957,7 @@
       </c>
       <c r="G3" s="7">
         <f>(C3-B3)*24</f>
-        <v>1.5</v>
+        <v>1.7499999999999991</v>
       </c>
       <c r="H3" s="1">
         <f>WEEKNUM(A3)</f>
@@ -923,12 +966,36 @@
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="8">
-        <v>3.2499999999999991</v>
+      <c r="K3" s="10">
+        <v>7.4999999999999973</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <f>DATE(2025,4,27)</f>
+        <v>45774</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7">
+        <f>(C4-B4)*24</f>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="H4" s="1">
+        <f>WEEKNUM(A4)</f>
+        <v>18</v>
+      </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>

</xml_diff>

<commit_message>
Update training goals in the README
</commit_message>
<xml_diff>
--- a/90_Misc/time_log.xlsx
+++ b/90_Misc/time_log.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/move_network/90_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4820C0EC-0BFC-814D-979F-57105D1A9A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65187712-F14A-9C4B-9B0A-33FD0E23361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="1340" windowWidth="20000" windowHeight="18760" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
+    <workbookView xWindow="13960" yWindow="1280" windowWidth="20000" windowHeight="18760" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId2"/>
+    <pivotCache cacheId="13" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -144,49 +144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -285,13 +243,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45787.814764120369" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45803.615188657408" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{162F23A0-815B-B34D-8D37-03DDB985FFFA}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Log"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-04-27T00:00:00" maxDate="2025-05-11T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-04-27T00:00:00" maxDate="2025-05-27T00:00:00"/>
     </cacheField>
     <cacheField name="Start" numFmtId="0">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T10:00:00" maxDate="1899-12-30T16:00:00"/>
@@ -309,12 +267,13 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.7499999999999991" maxValue="3"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.7499999999999991" maxValue="4.25"/>
     </cacheField>
     <cacheField name="Week" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="19" count="3">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="22" count="4">
         <n v="18"/>
         <n v="19"/>
+        <n v="22"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -370,13 +329,13 @@
     <x v="1"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2025-05-26T00:00:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <s v="move_network"/>
+    <n v="12"/>
+    <m/>
+    <n v="4.25"/>
     <x v="2"/>
   </r>
   <r>
@@ -387,114 +346,114 @@
     <m/>
     <m/>
     <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J1:K4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1638F497-0AD2-A544-8993-B6F54EFA0744}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J1:K5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -504,10 +463,11 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0" measureFilter="1">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -515,12 +475,15 @@
   <rowFields count="1">
     <field x="7"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -533,16 +496,16 @@
     <dataField name="Sum of Time" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="17">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="9">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="1">
@@ -551,10 +514,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -901,7 +864,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,11 +1006,11 @@
         <f>WEEKNUM(A4)</f>
         <v>19</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>10</v>
+      <c r="J4" s="9">
+        <v>22</v>
       </c>
       <c r="K4" s="10">
-        <v>9.4999999999999982</v>
+        <v>4.25</v>
       </c>
       <c r="L4" s="8"/>
     </row>
@@ -1076,11 +1039,39 @@
         <f>WEEKNUM(A5)</f>
         <v>19</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="J5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="10">
+        <v>13.749999999999998</v>
+      </c>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <f>DATE(2025,5,26)</f>
+        <v>45803</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7">
+        <f>(C6-B6)*24</f>
+        <v>4.25</v>
+      </c>
+      <c r="H6" s="1">
+        <f>WEEKNUM(A6)</f>
+        <v>22</v>
+      </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>

</xml_diff>

<commit_message>
Retrieve MSA data from bea
</commit_message>
<xml_diff>
--- a/90_Misc/time_log.xlsx
+++ b/90_Misc/time_log.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/move_network/90_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9936ECF-BFC7-B340-A736-E9690FD3ACAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F41E07-DE5F-0C40-B79D-B7961FA7C42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="2840" windowWidth="20000" windowHeight="18760" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
+    <workbookView xWindow="16420" yWindow="2200" windowWidth="20000" windowHeight="18760" xr2:uid="{62D59CB3-94D7-1B47-861E-7A4730E7CA93}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Hours Today</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -129,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -141,96 +150,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -329,13 +253,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45845.929779976854" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{29D7AB5D-F993-3442-9B2D-E7A726756DF3}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Notes" refreshedDate="45853.590616666668" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{29D7AB5D-F993-3442-9B2D-E7A726756DF3}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Log"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-04-27T00:00:00" maxDate="2025-07-08T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-04-27T00:00:00" maxDate="2025-07-16T00:00:00"/>
     </cacheField>
     <cacheField name="Start" numFmtId="0">
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1899-12-30T00:00:00" maxDate="1899-12-30T21:45:00"/>
@@ -356,7 +280,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="4.25"/>
     </cacheField>
     <cacheField name="Week" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="28" count="12">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="18" maxValue="29" count="13">
         <n v="18"/>
         <n v="19"/>
         <n v="20"/>
@@ -368,6 +292,7 @@
         <n v="26"/>
         <n v="27"/>
         <n v="28"/>
+        <n v="29"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -381,7 +306,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="19">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="28">
   <r>
     <d v="2025-04-27T00:00:00"/>
     <d v="1899-12-30T10:00:00"/>
@@ -563,21 +488,111 @@
     <x v="10"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2025-07-07T00:00:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="0.49999999999999956"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-08T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="1.9999999999999996"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-08T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="2.0000000000000009"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-09T00:00:00"/>
+    <d v="1899-12-30T07:30:00"/>
+    <d v="1899-12-30T08:15:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="0.75"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-09T00:00:00"/>
+    <d v="1899-12-30T09:00:00"/>
+    <d v="1899-12-30T09:30:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="0.49999999999999956"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-09T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="1.0000000000000004"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-09T00:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="1.9999999999999982"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-09T00:00:00"/>
+    <d v="1899-12-30T19:15:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="0.75"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2025-07-15T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <s v="move_network"/>
+    <n v="21"/>
+    <m/>
+    <n v="3.0000000000000013"/>
     <x v="11"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="12"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB11D5A6-3B11-6346-9F17-FBE554DAEFEF}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="K1:L14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB11D5A6-3B11-6346-9F17-FBE554DAEFEF}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="K1:L15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -587,7 +602,7 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="13">
+      <items count="14">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -600,6 +615,7 @@
         <item x="9"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -607,7 +623,7 @@
   <rowFields count="1">
     <field x="7"/>
   </rowFields>
-  <rowItems count="13">
+  <rowItems count="14">
     <i>
       <x/>
     </i>
@@ -644,6 +660,9 @@
     <i>
       <x v="11"/>
     </i>
+    <i>
+      <x v="12"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -655,58 +674,58 @@
     <dataField name="Sum of Time" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="16">
-    <format dxfId="31">
+    <format dxfId="15">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="13">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="9">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="7">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="2">
@@ -716,7 +735,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="2">
@@ -726,7 +745,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="7" count="1">
@@ -1076,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2CB818-6203-A04C-843B-4192B7E3207A}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,13 +1110,15 @@
     <col min="6" max="6" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="11" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1122,14 +1143,20 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <f>DATE(2025,4,27)</f>
         <v>45774</v>
@@ -1154,14 +1181,22 @@
         <f t="shared" ref="H2:H5" si="0">WEEKNUM(A2)</f>
         <v>18</v>
       </c>
+      <c r="I2" s="1">
+        <f ca="1">INT(A2=TODAY())*G2</f>
+        <v>0</v>
+      </c>
       <c r="K2" s="7">
         <v>18</v>
       </c>
       <c r="L2" s="8">
         <v>3.4999999999999982</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N2" s="1">
+        <f ca="1">SUM(I:I)</f>
+        <v>3.2500000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <f>DATE(2025,4,27)</f>
         <v>45774</v>
@@ -1186,6 +1221,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I27" ca="1" si="2">INT(A3=TODAY())*G3</f>
+        <v>0</v>
+      </c>
       <c r="K3" s="7">
         <v>19</v>
       </c>
@@ -1193,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <f>DATE(2025,5,10)</f>
         <v>45787</v>
@@ -1218,6 +1257,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="I4" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K4" s="7">
         <v>20</v>
       </c>
@@ -1225,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f>DATE(2025,5,10)</f>
         <v>45787</v>
@@ -1250,6 +1293,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="I5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K5" s="7">
         <v>21</v>
       </c>
@@ -1257,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <f>DATE(2025,5,15)</f>
         <v>45792</v>
@@ -1279,8 +1326,12 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6" si="2">WEEKNUM(A6)</f>
+        <f t="shared" ref="H6" si="3">WEEKNUM(A6)</f>
         <v>20</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="K6" s="7">
         <v>22</v>
@@ -1289,7 +1340,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <f>DATE(2025,5,20)</f>
         <v>45797</v>
@@ -1311,8 +1362,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7" si="3">WEEKNUM(A7)</f>
+        <f t="shared" ref="H7" si="4">WEEKNUM(A7)</f>
         <v>21</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
         <v>23</v>
@@ -1321,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f>DATE(2025,5,26)</f>
         <v>45803</v>
@@ -1346,6 +1401,10 @@
         <f>WEEKNUM(A8)</f>
         <v>22</v>
       </c>
+      <c r="I8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K8" s="7">
         <v>24</v>
       </c>
@@ -1353,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <f>DATE(2025,5,26+7)</f>
         <v>45810</v>
@@ -1378,6 +1437,10 @@
         <f>WEEKNUM(A9)</f>
         <v>23</v>
       </c>
+      <c r="I9" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K9" s="7">
         <v>25</v>
       </c>
@@ -1385,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <f>DATE(2025,5,26+14)</f>
         <v>45817</v>
@@ -1410,6 +1473,10 @@
         <f>WEEKNUM(A10)</f>
         <v>24</v>
       </c>
+      <c r="I10" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K10" s="7">
         <v>26</v>
       </c>
@@ -1417,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f>DATE(2025,6,15)</f>
         <v>45823</v>
@@ -1442,6 +1509,10 @@
         <f>WEEKNUM(A11)</f>
         <v>25</v>
       </c>
+      <c r="I11" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K11" s="7">
         <v>27</v>
       </c>
@@ -1449,7 +1520,7 @@
         <v>3.5000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <f>DATE(2025,6,15)</f>
         <v>45823</v>
@@ -1471,17 +1542,21 @@
         <v>2.7499999999999982</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" ref="H12" si="4">WEEKNUM(A12)</f>
+        <f t="shared" ref="H12" si="5">WEEKNUM(A12)</f>
         <v>25</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="K12" s="7">
         <v>28</v>
       </c>
       <c r="L12" s="8">
-        <v>6.7499999999999991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <f>DATE(2025,6,16)</f>
         <v>45824</v>
@@ -1503,15 +1578,21 @@
         <v>1.2500000000000009</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" ref="H13" si="5">WEEKNUM(A13)</f>
+        <f t="shared" ref="H13" si="6">WEEKNUM(A13)</f>
         <v>25</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>29</v>
+      </c>
+      <c r="L13" s="8">
+        <v>3.0000000000000013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f>DATE(2025,6,16+7)</f>
         <v>45831</v>
@@ -1533,17 +1614,19 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14" si="6">WEEKNUM(A14)</f>
+        <f t="shared" ref="H14" si="7">WEEKNUM(A14)</f>
         <v>26</v>
       </c>
+      <c r="I14" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
       <c r="K14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <f>DATE(2025,7,4)</f>
         <v>45842</v>
@@ -1565,11 +1648,21 @@
         <v>0.99999999999999911</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15" si="7">WEEKNUM(A15)</f>
+        <f t="shared" ref="H15" si="8">WEEKNUM(A15)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I15" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="1">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <f>DATE(2025,7,4)</f>
         <v>45842</v>
@@ -1591,11 +1684,15 @@
         <v>2.5000000000000018</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" ref="H16" si="8">WEEKNUM(A16)</f>
+        <f t="shared" ref="H16" si="9">WEEKNUM(A16)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f>DATE(2025,7,7)</f>
         <v>45845</v>
@@ -1613,15 +1710,22 @@
         <v>21</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" ref="G17" si="9">(C17-B17)*24</f>
+        <f t="shared" ref="G17" si="10">(C17-B17)*24</f>
         <v>1.9999999999999996</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17" si="10">WEEKNUM(A17)</f>
+        <f t="shared" ref="H17" si="11">WEEKNUM(A17)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <f>DATE(2025,7,7)</f>
         <v>45845</v>
@@ -1639,15 +1743,19 @@
         <v>21</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" ref="G18" si="11">(C18-B18)*24</f>
+        <f t="shared" ref="G18" si="12">(C18-B18)*24</f>
         <v>4.2499999999999982</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" ref="H18" si="12">WEEKNUM(A18)</f>
+        <f t="shared" ref="H18" si="13">WEEKNUM(A18)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f>DATE(2025,7,7)</f>
         <v>45845</v>
@@ -1665,12 +1773,286 @@
         <v>21</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" ref="G19" si="13">(C19-B19)*24</f>
+        <f t="shared" ref="G19" si="14">(C19-B19)*24</f>
         <v>0.50000000000000089</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19" si="14">WEEKNUM(A19)</f>
+        <f t="shared" ref="H19" si="15">WEEKNUM(A19)</f>
         <v>28</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <f>DATE(2025,7,7)</f>
+        <v>45845</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" ref="G20" si="16">(C20-B20)*24</f>
+        <v>0.49999999999999956</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20" si="17">WEEKNUM(A20)</f>
+        <v>28</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <f>DATE(2025,7,8)</f>
+        <v>45846</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>21</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" ref="G21" si="18">(C21-B21)*24</f>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" ref="H21" si="19">WEEKNUM(A21)</f>
+        <v>28</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <f>DATE(2025,7,8)</f>
+        <v>45846</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>21</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" ref="G22" si="20">(C22-B22)*24</f>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" ref="H22" si="21">WEEKNUM(A22)</f>
+        <v>28</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <f>DATE(2025,7,9)</f>
+        <v>45847</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.3125</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.34375</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>21</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" ref="G23" si="22">(C23-B23)*24</f>
+        <v>0.75</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23" si="23">WEEKNUM(A23)</f>
+        <v>28</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <f>DATE(2025,7,9)</f>
+        <v>45847</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>21</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" ref="G24" si="24">(C24-B24)*24</f>
+        <v>0.49999999999999956</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" ref="H24" si="25">WEEKNUM(A24)</f>
+        <v>28</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <f>DATE(2025,7,9)</f>
+        <v>45847</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>21</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" ref="G25" si="26">(C25-B25)*24</f>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25" si="27">WEEKNUM(A25)</f>
+        <v>28</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <f>DATE(2025,7,9)</f>
+        <v>45847</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>21</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" ref="G26" si="28">(C26-B26)*24</f>
+        <v>1.9999999999999982</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" ref="H26" si="29">WEEKNUM(A26)</f>
+        <v>28</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <f>DATE(2025,7,9)</f>
+        <v>45847</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2">
+        <v>21</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" ref="G27" si="30">(C27-B27)*24</f>
+        <v>0.75</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27" si="31">WEEKNUM(A27)</f>
+        <v>28</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <f>DATE(2025,7,15)</f>
+        <v>45853</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2">
+        <v>21</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" ref="G28" si="32">(C28-B28)*24</f>
+        <v>3.2500000000000004</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" ref="H28" si="33">WEEKNUM(A28)</f>
+        <v>29</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ref="I28" ca="1" si="34">INT(A28=TODAY())*G28</f>
+        <v>3.2500000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>